<commit_message>
Included planning details on excel file
</commit_message>
<xml_diff>
--- a/OTB/Mapeo OTB.xlsx
+++ b/OTB/Mapeo OTB.xlsx
@@ -1,30 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src_mad\TDW_Analytics\ADOC_PBIs\OTB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E847FB-124E-48C4-961A-E42D46F19AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6EF02D-E72D-45B8-AF32-9817E0E988A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9F3BD3-5836-4EDE-80E9-55945817595E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
-    <sheet name="Base OTB" sheetId="1" r:id="rId2"/>
+    <sheet name="Detalle de acciones" sheetId="4" r:id="rId1"/>
+    <sheet name="Origenes" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Base OTB" sheetId="1" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Base OTB'!$A$1:$F$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Base OTB'!$A$1:$F$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="42" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -68,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="137">
   <si>
     <t>Expressions</t>
   </si>
@@ -374,6 +377,111 @@
   </si>
   <si>
     <t>SQL - Server Dev</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>Arribos Planner</t>
+  </si>
+  <si>
+    <t>LAP MARCAS</t>
+  </si>
+  <si>
+    <t>LAP PLANNER</t>
+  </si>
+  <si>
+    <t>Fase</t>
+  </si>
+  <si>
+    <t>Acciones</t>
+  </si>
+  <si>
+    <t>Fase 1</t>
+  </si>
+  <si>
+    <t>ALMACENES , Arribos , Arribos sql original , DatosArticulos , Jerarquía Base , UltimaFecha OTB , Agrupacion_Marcas , ArticuloProveedor</t>
+  </si>
+  <si>
+    <t>EKPO</t>
+  </si>
+  <si>
+    <t>OTB / Ventas</t>
+  </si>
+  <si>
+    <t>Adelantos L1 , Arribos , Arribos Planner , Base L1 , Base Planes , BaseTipoPlanes , Equivalentes , Inventario TGT , Inventario TGT NOS , LAP MARCAS , LAP PLANNER , Reservas L1</t>
+  </si>
+  <si>
+    <t>Fase 0</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Garantizar que cada origen de datos detallado está a nivel de MATNR y SK_Tienda, para poder realizar el mapeo a nivel de dimensionales</t>
+  </si>
+  <si>
+    <t>Fase 2</t>
+  </si>
+  <si>
+    <t>Eliminar agregaciones de archivos de Sharepoint ( 23 fuentes )</t>
+  </si>
+  <si>
+    <t>Carga de datos a un dataflow Ge1 desde SQL Server ( 8 fuentes )</t>
+  </si>
+  <si>
+    <t>cargar desde PowerBI ( SSAS ) ( 1 fuente )</t>
+  </si>
+  <si>
+    <t>Cargar desde Sharepoint ( 23 fuentes )</t>
+  </si>
+  <si>
+    <t>Fase 3</t>
+  </si>
+  <si>
+    <t>Carga de tablas base a PowerBI</t>
+  </si>
+  <si>
+    <t>Fase 4</t>
+  </si>
+  <si>
+    <t>Creación de relaciones desde hechos a dimensionales globales</t>
+  </si>
+  <si>
+    <t>Dimensiones a crear: Productos, Tiendas, Almacenes, Fechas</t>
+  </si>
+  <si>
+    <t>Fase 5</t>
+  </si>
+  <si>
+    <t>Replicación de métricas dentro de PowerBI</t>
+  </si>
+  <si>
+    <t>Tiempo</t>
+  </si>
+  <si>
+    <t>cargar desde SQL Server / Big Query ( 10 fuentes )</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>TDW</t>
+  </si>
+  <si>
+    <t>ADOC</t>
+  </si>
+  <si>
+    <t>Se debe trabajar en conjunto para replicar todos los cálculos del OTB actual, al optimizado</t>
+  </si>
+  <si>
+    <t>Preparación de datos a nivel de MATNT, SK_TIENDA - SQL Server (10)</t>
+  </si>
+  <si>
+    <t>Preparación de datos a nivel de MATNT, SK_TIENDA - Big Query (2)</t>
+  </si>
+  <si>
+    <t>Preparación de datos a nivel de MATNT, SK_TIENDA - Sharepoint (23)</t>
   </si>
 </sst>
 </file>
@@ -409,7 +517,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +533,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -495,14 +615,475 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="97">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -522,45 +1103,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -574,6 +1116,24 @@
       <font>
         <b/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
     </dxf>
     <dxf>
       <font>
@@ -592,21 +1152,6 @@
         <color theme="0"/>
         <family val="2"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -631,6 +1176,7 @@
       <sheetName val="Hoja1"/>
     </sheetNames>
     <definedNames>
+      <definedName name="Array_Concat"/>
       <definedName name="Array_to_Dax_Strings"/>
     </definedNames>
     <sheetDataSet>
@@ -721,7 +1267,24 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Dependencias" numFmtId="0">
-      <sharedItems containsBlank="1"/>
+      <sharedItems containsBlank="1" count="16">
+        <m/>
+        <s v="Adelantos L1, Equivalentes, Jerarquía Base"/>
+        <s v="Agrupacion_Marcas"/>
+        <s v="LAP Planner 1, LAP Planner 2, LAP Planner 3, LAP Planner 4, Base L1"/>
+        <s v="Arribos Planner 1, Arribos Planner 2, Arribos Planner 3, Arribos Planner 4, Jerarquía Base"/>
+        <s v="LAP PAR2, LAP INTER, LAP ADOC"/>
+        <s v="Base Planes"/>
+        <s v="ALMACENES, Agrupacion_Marcas"/>
+        <s v="Agrupacion_Marcas, LAP Base"/>
+        <s v="ArticuloProveedor"/>
+        <s v="Agrupacion_Marcas, Arribos Ajustados"/>
+        <s v="Agrupacion_Marcas, Inventario TGT NOS"/>
+        <s v="LAP Planner 1, LAP Planner 2, LAP Planner 3, LAP Planner 4, LAP Open"/>
+        <s v="Arribos, Plan Final, Reservas L1, Arribos ADOC, Arribos PAR2, Arribos INTER, LAP, Inventario TGT, LAP NOS, Agrupacion_Marcas, EKPO import"/>
+        <s v="UltimaFecha OTB"/>
+        <s v="Plan Final"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="SOURCE" numFmtId="0">
       <sharedItems containsBlank="1" count="23">
@@ -762,13 +1325,98 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Mario Alvarado" refreshedDate="45855.43597997685" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="56" xr:uid="{2E192E80-B54D-4ACE-9FE0-553C09D70F15}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="K2:M58" sheet="Base OTB"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Object" numFmtId="0">
+      <sharedItems count="26">
+        <s v="Reservas L1"/>
+        <s v="Arribos Planner 1"/>
+        <s v="Arribos Planner 2"/>
+        <s v="Arribos Planner 3"/>
+        <s v="Arribos Planner 4"/>
+        <s v="LAP ADOC"/>
+        <s v="LAP PAR2"/>
+        <s v="LAP INTER"/>
+        <s v="Arribos ADOC"/>
+        <s v="Arribos PAR2"/>
+        <s v="Arribos INTER"/>
+        <s v="LAP Base"/>
+        <s v="Arribos Ajustados"/>
+        <s v="LAP"/>
+        <s v="Plan Final"/>
+        <s v="EKPO import"/>
+        <s v="Jerarquía Base"/>
+        <s v="Inventario TGT NOS"/>
+        <s v="Arribos"/>
+        <s v="Inventario TGT"/>
+        <s v="LAP NOS"/>
+        <s v="LAP Open"/>
+        <s v="OTB"/>
+        <s v="OTB Max Fecha"/>
+        <s v="Plan Max Año"/>
+        <s v="Planes"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Dependency" numFmtId="0">
+      <sharedItems count="33">
+        <s v="Adelantos L1"/>
+        <s v="Equivalentes"/>
+        <s v="Jerarquía Base"/>
+        <s v="Agrupacion_Marcas"/>
+        <s v="LAP Planner 1"/>
+        <s v="LAP Planner 2"/>
+        <s v="LAP Planner 3"/>
+        <s v="LAP Planner 4"/>
+        <s v="Base L1"/>
+        <s v="Arribos Planner 1"/>
+        <s v="Arribos Planner 2"/>
+        <s v="Arribos Planner 3"/>
+        <s v="Arribos Planner 4"/>
+        <s v="LAP PAR2"/>
+        <s v="LAP INTER"/>
+        <s v="LAP ADOC"/>
+        <s v="Base Planes"/>
+        <s v="ALMACENES"/>
+        <s v="LAP Base"/>
+        <s v="Arribos Ajustados"/>
+        <s v="Inventario TGT NOS"/>
+        <s v="LAP Open"/>
+        <s v="Arribos"/>
+        <s v="Plan Final"/>
+        <s v="Reservas L1"/>
+        <s v="Arribos ADOC"/>
+        <s v="Arribos PAR2"/>
+        <s v="Arribos INTER"/>
+        <s v="LAP"/>
+        <s v="Inventario TGT"/>
+        <s v="LAP NOS"/>
+        <s v="EKPO import"/>
+        <s v="UltimaFecha OTB"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="0" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="49">
   <r>
     <s v="Expressions"/>
     <x v="0"/>
     <x v="0"/>
-    <m/>
+    <x v="0"/>
     <x v="0"/>
     <n v="0"/>
   </r>
@@ -776,7 +1424,7 @@
     <s v="Expressions"/>
     <x v="1"/>
     <x v="1"/>
-    <m/>
+    <x v="0"/>
     <x v="1"/>
     <n v="1"/>
   </r>
@@ -784,7 +1432,7 @@
     <s v="Expressions"/>
     <x v="2"/>
     <x v="2"/>
-    <s v="Adelantos L1, Equivalentes, Jerarquía Base"/>
+    <x v="1"/>
     <x v="2"/>
     <n v="1"/>
   </r>
@@ -792,7 +1440,7 @@
     <s v="Expressions"/>
     <x v="3"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
     <x v="3"/>
     <n v="1"/>
   </r>
@@ -800,7 +1448,7 @@
     <s v="Expressions"/>
     <x v="4"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
     <x v="2"/>
     <n v="1"/>
   </r>
@@ -808,7 +1456,7 @@
     <s v="Expressions"/>
     <x v="5"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
     <x v="4"/>
     <n v="2"/>
   </r>
@@ -816,7 +1464,7 @@
     <s v="Expressions"/>
     <x v="6"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
     <x v="5"/>
     <n v="2"/>
   </r>
@@ -824,7 +1472,7 @@
     <s v="Expressions"/>
     <x v="7"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
     <x v="6"/>
     <n v="2"/>
   </r>
@@ -832,7 +1480,7 @@
     <s v="Expressions"/>
     <x v="8"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
     <x v="7"/>
     <n v="1"/>
   </r>
@@ -840,7 +1488,7 @@
     <s v="Expressions"/>
     <x v="9"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="8"/>
     <n v="1"/>
   </r>
@@ -848,7 +1496,7 @@
     <s v="Expressions"/>
     <x v="10"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="4"/>
     <n v="1"/>
   </r>
@@ -856,7 +1504,7 @@
     <s v="Expressions"/>
     <x v="11"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="5"/>
     <n v="1"/>
   </r>
@@ -864,7 +1512,7 @@
     <s v="Expressions"/>
     <x v="12"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="6"/>
     <n v="1"/>
   </r>
@@ -872,7 +1520,7 @@
     <s v="Expressions"/>
     <x v="13"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="9"/>
     <n v="1"/>
   </r>
@@ -880,7 +1528,7 @@
     <s v="Expressions"/>
     <x v="14"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="10"/>
     <n v="1"/>
   </r>
@@ -888,7 +1536,7 @@
     <s v="Expressions"/>
     <x v="15"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="11"/>
     <n v="1"/>
   </r>
@@ -896,7 +1544,7 @@
     <s v="Expressions"/>
     <x v="16"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="9"/>
     <n v="1"/>
   </r>
@@ -904,7 +1552,7 @@
     <s v="Expressions"/>
     <x v="17"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="10"/>
     <n v="1"/>
   </r>
@@ -912,7 +1560,7 @@
     <s v="Expressions"/>
     <x v="18"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="11"/>
     <n v="1"/>
   </r>
@@ -920,7 +1568,7 @@
     <s v="Expressions"/>
     <x v="19"/>
     <x v="3"/>
-    <s v="LAP Planner 1, LAP Planner 2, LAP Planner 3, LAP Planner 4, Base L1"/>
+    <x v="3"/>
     <x v="0"/>
     <n v="1"/>
   </r>
@@ -928,7 +1576,7 @@
     <s v="Expressions"/>
     <x v="20"/>
     <x v="3"/>
-    <s v="Arribos Planner 1, Arribos Planner 2, Arribos Planner 3, Arribos Planner 4, Jerarquía Base"/>
+    <x v="4"/>
     <x v="0"/>
     <n v="1"/>
   </r>
@@ -936,7 +1584,7 @@
     <s v="Expressions"/>
     <x v="21"/>
     <x v="3"/>
-    <s v="LAP PAR2, LAP INTER, LAP ADOC"/>
+    <x v="5"/>
     <x v="0"/>
     <n v="1"/>
   </r>
@@ -944,7 +1592,7 @@
     <s v="Expressions"/>
     <x v="22"/>
     <x v="3"/>
-    <s v="Base Planes"/>
+    <x v="6"/>
     <x v="0"/>
     <n v="2"/>
   </r>
@@ -952,7 +1600,7 @@
     <s v="Expressions"/>
     <x v="23"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
     <x v="12"/>
     <n v="2"/>
   </r>
@@ -960,7 +1608,7 @@
     <s v="Expressions"/>
     <x v="24"/>
     <x v="1"/>
-    <m/>
+    <x v="0"/>
     <x v="13"/>
     <n v="1"/>
   </r>
@@ -968,7 +1616,7 @@
     <s v="Expressions"/>
     <x v="25"/>
     <x v="4"/>
-    <s v="ALMACENES, Agrupacion_Marcas"/>
+    <x v="7"/>
     <x v="14"/>
     <n v="1"/>
   </r>
@@ -976,7 +1624,7 @@
     <s v="Expressions"/>
     <x v="26"/>
     <x v="1"/>
-    <s v="Agrupacion_Marcas, LAP Base"/>
+    <x v="8"/>
     <x v="15"/>
     <n v="2"/>
   </r>
@@ -984,7 +1632,7 @@
     <s v="Expressions"/>
     <x v="27"/>
     <x v="5"/>
-    <m/>
+    <x v="0"/>
     <x v="16"/>
     <n v="17"/>
   </r>
@@ -992,7 +1640,7 @@
     <s v="Expressions"/>
     <x v="28"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="17"/>
     <n v="1"/>
   </r>
@@ -1000,7 +1648,7 @@
     <s v="Expressions"/>
     <x v="29"/>
     <x v="1"/>
-    <m/>
+    <x v="0"/>
     <x v="15"/>
     <n v="0"/>
   </r>
@@ -1008,7 +1656,7 @@
     <s v="Expressions"/>
     <x v="30"/>
     <x v="3"/>
-    <s v="ArticuloProveedor"/>
+    <x v="9"/>
     <x v="0"/>
     <n v="0"/>
   </r>
@@ -1016,7 +1664,7 @@
     <s v="Tables"/>
     <x v="31"/>
     <x v="6"/>
-    <m/>
+    <x v="0"/>
     <x v="0"/>
     <n v="0"/>
   </r>
@@ -1024,7 +1672,7 @@
     <s v="Tables"/>
     <x v="32"/>
     <x v="0"/>
-    <m/>
+    <x v="0"/>
     <x v="0"/>
     <n v="0"/>
   </r>
@@ -1032,7 +1680,7 @@
     <s v="Tables"/>
     <x v="33"/>
     <x v="1"/>
-    <s v="Agrupacion_Marcas, Arribos Ajustados"/>
+    <x v="10"/>
     <x v="15"/>
     <n v="1"/>
   </r>
@@ -1040,7 +1688,7 @@
     <s v="Tables"/>
     <x v="34"/>
     <x v="1"/>
-    <m/>
+    <x v="0"/>
     <x v="15"/>
     <n v="0"/>
   </r>
@@ -1048,7 +1696,7 @@
     <s v="Tables"/>
     <x v="35"/>
     <x v="7"/>
-    <m/>
+    <x v="0"/>
     <x v="18"/>
     <n v="0"/>
   </r>
@@ -1056,7 +1704,7 @@
     <s v="Tables"/>
     <x v="36"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
     <x v="12"/>
     <n v="0"/>
   </r>
@@ -1064,7 +1712,7 @@
     <s v="Tables"/>
     <x v="37"/>
     <x v="6"/>
-    <m/>
+    <x v="0"/>
     <x v="0"/>
     <n v="0"/>
   </r>
@@ -1072,7 +1720,7 @@
     <s v="Tables"/>
     <x v="38"/>
     <x v="8"/>
-    <m/>
+    <x v="0"/>
     <x v="19"/>
     <n v="0"/>
   </r>
@@ -1080,7 +1728,7 @@
     <s v="Tables"/>
     <x v="39"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas, Inventario TGT NOS"/>
+    <x v="11"/>
     <x v="20"/>
     <n v="1"/>
   </r>
@@ -1088,7 +1736,7 @@
     <s v="Tables"/>
     <x v="40"/>
     <x v="3"/>
-    <s v="LAP Planner 1, LAP Planner 2, LAP Planner 3, LAP Planner 4, LAP Open"/>
+    <x v="12"/>
     <x v="0"/>
     <n v="1"/>
   </r>
@@ -1096,7 +1744,7 @@
     <s v="Tables"/>
     <x v="41"/>
     <x v="2"/>
-    <s v="Agrupacion_Marcas"/>
+    <x v="2"/>
     <x v="21"/>
     <n v="1"/>
   </r>
@@ -1104,7 +1752,7 @@
     <s v="Tables"/>
     <x v="42"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
     <x v="22"/>
     <n v="2"/>
   </r>
@@ -1112,7 +1760,7 @@
     <s v="Tables"/>
     <x v="43"/>
     <x v="8"/>
-    <s v="Arribos, Plan Final, Reservas L1, Arribos ADOC, Arribos PAR2, Arribos INTER, LAP, Inventario TGT, LAP NOS, Agrupacion_Marcas, EKPO import"/>
+    <x v="13"/>
     <x v="19"/>
     <n v="0"/>
   </r>
@@ -1120,7 +1768,7 @@
     <s v="Tables"/>
     <x v="44"/>
     <x v="3"/>
-    <s v="UltimaFecha OTB"/>
+    <x v="14"/>
     <x v="0"/>
     <n v="0"/>
   </r>
@@ -1128,7 +1776,7 @@
     <s v="Tables"/>
     <x v="45"/>
     <x v="3"/>
-    <s v="Plan Final"/>
+    <x v="15"/>
     <x v="0"/>
     <n v="0"/>
   </r>
@@ -1136,7 +1784,7 @@
     <s v="Tables"/>
     <x v="46"/>
     <x v="3"/>
-    <s v="Base Planes"/>
+    <x v="6"/>
     <x v="0"/>
     <n v="0"/>
   </r>
@@ -1144,7 +1792,7 @@
     <s v="Tables"/>
     <x v="47"/>
     <x v="6"/>
-    <m/>
+    <x v="0"/>
     <x v="0"/>
     <n v="0"/>
   </r>
@@ -1152,16 +1800,301 @@
     <s v="Tables"/>
     <x v="48"/>
     <x v="6"/>
-    <m/>
+    <x v="0"/>
     <x v="0"/>
     <n v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="56">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="7"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="8"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="9"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="10"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="11"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="12"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="13"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="14"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="15"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="16"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="17"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="18"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="19"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="20"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="7"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="21"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="22"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="23"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="24"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="25"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="26"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="27"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="28"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="29"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="30"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="31"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="32"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="23"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="16"/>
+    <n v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{852028B4-D9E3-492F-9BC2-580018DE1910}" name="TablaDinámica1" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A3:D41" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{852028B4-D9E3-492F-9BC2-580018DE1910}" name="TablaDinámica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A3:D38" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="6">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -1217,14 +2150,14 @@
         <item x="1"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
       <items count="14">
         <item m="1" x="12"/>
         <item m="1" x="9"/>
         <item x="8"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="0"/>
+        <item h="1" sd="0" x="6"/>
+        <item h="1" sd="0" x="3"/>
+        <item h="1" sd="0" x="0"/>
         <item m="1" x="13"/>
         <item m="1" x="11"/>
         <item m="1" x="10"/>
@@ -1235,7 +2168,26 @@
         <item x="7"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="16">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="15"/>
+        <item x="14"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="23">
         <item x="16"/>
@@ -1270,7 +2222,7 @@
     <field x="1"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="38">
+  <rowItems count="35">
     <i>
       <x v="2"/>
       <x v="23"/>
@@ -1279,15 +2231,6 @@
     <i r="1">
       <x v="39"/>
       <x v="3"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
     </i>
     <i>
       <x v="9"/>
@@ -1432,9 +2375,9 @@
   <dataFields count="1">
     <dataField name="Cuenta de Dependencias" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="21">
-    <format dxfId="20">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="A256" fieldPosition="0">
+  <formats count="97">
+    <format dxfId="82">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
             <x v="3"/>
@@ -1442,8 +2385,8 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="A256" fieldPosition="0">
+    <format dxfId="83">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
             <x v="4"/>
@@ -1451,8 +2394,8 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="A256" fieldPosition="0">
+    <format dxfId="84">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
             <x v="5"/>
@@ -1460,7 +2403,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1469,7 +2412,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1478,7 +2421,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1487,7 +2430,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1496,7 +2439,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1505,7 +2448,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1514,7 +2457,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1523,7 +2466,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1532,7 +2475,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1541,7 +2484,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1550,7 +2493,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1559,7 +2502,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -1568,56 +2511,1237 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="81">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    </format>
+    <format dxfId="80">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="79">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="23"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="78">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="77">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="76">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="75">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="74">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="73">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="72">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="71">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="70">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="13"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="16"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="68">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="17"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="16"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="67">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="18"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="16"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="66">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="22"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="65">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="25"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="26"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="63">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="29"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="31"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="61">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="33"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="60">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="34"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="59">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="35"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="58">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="57">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="37"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="56">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="38"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="55">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="45"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="54">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="21"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="20"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="53">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="52">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="51">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="14"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="50">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="20"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="49">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="27"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="48">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="48"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="47">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="46">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="15"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="13"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="21"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="45">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="4" selected="0">
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="4" selected="0">
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="44">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="4">
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="43">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="42">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="41">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="40">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="13"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="39">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="3" selected="0">
+            <x v="6"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="3" selected="0">
+            <x v="17"/>
+            <x v="18"/>
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="3">
+            <x v="6"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="37">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="35">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="4" selected="0">
+            <x v="29"/>
+            <x v="31"/>
+            <x v="33"/>
+            <x v="34"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="4" selected="0">
+            <x v="11"/>
+            <x v="17"/>
+            <x v="18"/>
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="4">
+            <x v="29"/>
+            <x v="31"/>
+            <x v="33"/>
+            <x v="34"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="29"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="31"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="33"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="34"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="4" selected="0">
+            <x v="35"/>
+            <x v="36"/>
+            <x v="37"/>
+            <x v="38"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="4" selected="0">
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="35"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="37"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="38"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="4" selected="0">
+            <x v="35"/>
+            <x v="36"/>
+            <x v="37"/>
+            <x v="38"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="4" selected="0">
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="4">
+            <x v="35"/>
+            <x v="36"/>
+            <x v="37"/>
+            <x v="38"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="35"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="37"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="38"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="6">
+            <x v="4"/>
+            <x v="5"/>
+            <x v="14"/>
+            <x v="20"/>
+            <x v="27"/>
+            <x v="48"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1">
+            <x v="15"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="8" selected="0">
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="14"/>
+            <x v="15"/>
+            <x v="20"/>
+            <x v="27"/>
+            <x v="48"/>
+          </reference>
+          <reference field="2" count="3" selected="0">
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+          </reference>
+          <reference field="4" count="5" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="21"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="6">
+            <x v="4"/>
+            <x v="5"/>
+            <x v="14"/>
+            <x v="20"/>
+            <x v="27"/>
+            <x v="48"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1">
+            <x v="15"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="14"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="20"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="27"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="5">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="A256" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="48"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
             <x v="3"/>
           </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="4">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="A256" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1">
-            <x v="4"/>
+          <reference field="2" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="3">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="A256" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1">
-            <x v="5"/>
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="15"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="13"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="21"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="2">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1">
-            <x v="3"/>
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="21"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="20"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1">
-            <x v="4"/>
+        <references count="2">
+          <reference field="1" count="1">
+            <x v="21"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="10"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1">
-            <x v="5"/>
+        <references count="3">
+          <reference field="1" count="1" selected="0">
+            <x v="21"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="20"/>
           </reference>
         </references>
       </pivotArea>
@@ -1630,6 +3754,351 @@
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5078180F-72D8-48E0-98A7-D9545285730B}" name="TablaDinámica1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:A86" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="27">
+        <item x="18"/>
+        <item x="8"/>
+        <item x="12"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="15"/>
+        <item x="19"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="13"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="6"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="14"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="34">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="17"/>
+        <item x="22"/>
+        <item x="25"/>
+        <item x="19"/>
+        <item x="27"/>
+        <item x="26"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="16"/>
+        <item x="31"/>
+        <item x="1"/>
+        <item x="29"/>
+        <item x="20"/>
+        <item x="2"/>
+        <item x="28"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item x="14"/>
+        <item x="30"/>
+        <item x="21"/>
+        <item x="13"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="32"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="83">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
+    </i>
+    <i r="1">
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -1951,403 +4420,1136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5B7ABC-F99E-48E7-9D1D-16B87ABF969B}">
-  <dimension ref="A3:D41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124E7CE5-828D-4070-99A8-F619707FCA09}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="195.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="156.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="22"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="25">
+        <v>20</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="25">
+        <v>4</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="25">
+        <v>72</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25">
+        <v>48</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="25">
+        <v>16</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="25">
+        <v>2</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="25">
+        <v>20</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="25">
+        <v>46</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25">
+        <v>8</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="25">
+        <v>2</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="25">
+        <v>96</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f>SUM(D2:D12)</f>
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5B7ABC-F99E-48E7-9D1D-16B87ABF969B}">
+  <dimension ref="A3:G40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="15" t="s">
         <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7">
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" t="str">
+        <f>B6</f>
+        <v>Adelantos L1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="20">
+        <v>1</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="20">
+        <v>1</v>
+      </c>
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="20">
+        <v>1</v>
+      </c>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="20">
+        <v>1</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="20">
+        <v>1</v>
+      </c>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="20">
+        <v>1</v>
+      </c>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="20">
+        <v>1</v>
+      </c>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" t="str">
+        <f t="shared" ref="E14:E19" si="0">B14</f>
+        <v>Base L1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>Base Planes</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>BaseTipoPlanes</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>Equivalentes</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>Inventario TGT</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="14">
+        <v>1</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>Inventario TGT NOS</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="20">
+        <v>1</v>
+      </c>
+      <c r="E21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="20">
+        <v>1</v>
+      </c>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="20">
+        <v>1</v>
+      </c>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="14">
+        <v>1</v>
+      </c>
+      <c r="E28" t="str">
+        <f>B28</f>
+        <v>Reservas L1</v>
+      </c>
+      <c r="G28" t="str" cm="1">
+        <f t="array" ref="G28">[1]!Array_Concat(E6:E28)</f>
+        <v>Adelantos L1 , Arribos ,  ,  , Arribos Planner ,  ,  ,  , Base L1 , Base Planes , BaseTipoPlanes , Equivalentes , Inventario TGT , Inventario TGT NOS , LAP MARCAS ,  ,  ,  , LAP PLANNER ,  ,  ,  , Reservas L1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="20"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="20"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="20"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="20"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="20"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="20"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38"/>
+      <c r="D38" s="14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="str" cm="1">
+        <f t="array" ref="B40">[1]!Array_Concat(B30:B37)</f>
+        <v>ALMACENES , Arribos , Arribos sql original , DatosArticulos , Jerarquía Base , UltimaFecha OTB , Agrupacion_Marcas , ArticuloProveedor</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="E20:E23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505DC2B7-B020-42CA-BF2D-6937C848078A}">
+  <dimension ref="A3:A86"/>
+  <sheetViews>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C37" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="D41">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2355,13 +5557,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E28149-3C6E-4E25-8BDE-5C425769E8BE}">
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2705,7 +5907,7 @@
       </c>
       <c r="H10" t="str" cm="1">
         <f t="array" ref="H10">[1]!Array_to_Dax_Strings(B10,D10)</f>
-        <v xml:space="preserve">{ "Arribos ADOC" , "1" } </v>
+        <v xml:space="preserve">{ "Base L1" , "" } </v>
       </c>
       <c r="I10" t="s">
         <v>92</v>

</xml_diff>